<commit_message>
cierre 20 may 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #05  MAYO  2022/CREDITOS  4 CARNES   ZAVALETA   MAYO    2022.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #05  MAYO  2022/CREDITOS  4 CARNES   ZAVALETA   MAYO    2022.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="50">
   <si>
     <t>REMISION</t>
   </si>
@@ -304,6 +304,9 @@
   <si>
     <t xml:space="preserve">PROSUBCA </t>
   </si>
+  <si>
+    <t>OK</t>
+  </si>
 </sst>
 </file>
 
@@ -315,7 +318,7 @@
     <numFmt numFmtId="165" formatCode="[$-C0A]d\-mmm\-yy;@"/>
     <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -495,6 +498,14 @@
       <b/>
       <sz val="13"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFCC0099"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -848,7 +859,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="175">
+  <cellXfs count="176">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1172,6 +1183,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1247,10 +1261,10 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFCC0099"/>
       <color rgb="FF0000FF"/>
       <color rgb="FFCC99FF"/>
       <color rgb="FF990033"/>
-      <color rgb="FFCC0099"/>
       <color rgb="FF00FF00"/>
       <color rgb="FF66FFFF"/>
       <color rgb="FF9966FF"/>
@@ -2665,24 +2679,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="158" t="s">
+      <c r="B1" s="159" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="159"/>
-      <c r="D1" s="159"/>
-      <c r="E1" s="159"/>
-      <c r="F1" s="160"/>
+      <c r="C1" s="160"/>
+      <c r="D1" s="160"/>
+      <c r="E1" s="160"/>
+      <c r="F1" s="161"/>
       <c r="H1" s="2"/>
     </row>
     <row r="2" spans="1:8" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
-      <c r="B2" s="153" t="s">
+      <c r="B2" s="154" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="153"/>
-      <c r="D2" s="153"/>
-      <c r="E2" s="153"/>
-      <c r="F2" s="153"/>
+      <c r="C2" s="154"/>
+      <c r="D2" s="154"/>
+      <c r="E2" s="154"/>
+      <c r="F2" s="154"/>
       <c r="G2" s="5"/>
       <c r="H2" s="2"/>
     </row>
@@ -3828,12 +3842,12 @@
     <row r="55" spans="1:8" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B55" s="37"/>
       <c r="C55" s="2"/>
-      <c r="D55" s="154">
+      <c r="D55" s="155">
         <f>D51-F51</f>
         <v>0</v>
       </c>
-      <c r="E55" s="155"/>
-      <c r="F55" s="156"/>
+      <c r="E55" s="156"/>
+      <c r="F55" s="157"/>
       <c r="H55" s="2"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
@@ -3847,11 +3861,11 @@
     <row r="57" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B57" s="37"/>
       <c r="C57" s="2"/>
-      <c r="D57" s="157" t="s">
+      <c r="D57" s="158" t="s">
         <v>8</v>
       </c>
-      <c r="E57" s="157"/>
-      <c r="F57" s="157"/>
+      <c r="E57" s="158"/>
+      <c r="F57" s="158"/>
       <c r="H57" s="2"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
@@ -3960,38 +3974,39 @@
   <sheetPr>
     <tabColor rgb="FFC00000"/>
   </sheetPr>
-  <dimension ref="A1:E62"/>
+  <dimension ref="A1:F62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="11.42578125" style="123"/>
     <col min="3" max="3" width="14.85546875" style="149" customWidth="1"/>
     <col min="4" max="4" width="16.7109375" style="124" customWidth="1"/>
     <col min="5" max="5" width="14.140625" style="123" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="11.42578125" style="123"/>
+    <col min="6" max="6" width="11.42578125" style="153"/>
+    <col min="7" max="16384" width="11.42578125" style="123"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="164"/>
-      <c r="B1" s="165"/>
-      <c r="C1" s="165"/>
-      <c r="D1" s="165"/>
-      <c r="E1" s="165"/>
-    </row>
-    <row r="2" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="166" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="165"/>
+      <c r="B1" s="166"/>
+      <c r="C1" s="166"/>
+      <c r="D1" s="166"/>
+      <c r="E1" s="166"/>
+    </row>
+    <row r="2" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="167" t="s">
         <v>43</v>
       </c>
-      <c r="B2" s="167"/>
-      <c r="C2" s="167"/>
-      <c r="D2" s="167"/>
-      <c r="E2" s="167"/>
-    </row>
-    <row r="3" spans="1:5" ht="33.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="168"/>
+      <c r="C2" s="168"/>
+      <c r="D2" s="168"/>
+      <c r="E2" s="168"/>
+    </row>
+    <row r="3" spans="1:6" ht="33.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="142" t="s">
         <v>44</v>
       </c>
@@ -4005,7 +4020,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="140">
         <v>44690</v>
       </c>
@@ -4019,8 +4034,11 @@
         <f>D4</f>
         <v>67500</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F4" s="153" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="89">
         <v>44691</v>
       </c>
@@ -4035,7 +4053,7 @@
         <v>142189</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="89">
         <v>44692</v>
       </c>
@@ -4050,7 +4068,7 @@
         <v>207018</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="89">
         <v>44693</v>
       </c>
@@ -4065,7 +4083,7 @@
         <v>247093</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="89">
         <v>44694</v>
       </c>
@@ -4080,7 +4098,7 @@
         <v>303144</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="89">
         <v>44695</v>
       </c>
@@ -4095,7 +4113,7 @@
         <v>346594</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="89">
         <v>44696</v>
       </c>
@@ -4110,7 +4128,7 @@
         <v>398929</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="89"/>
       <c r="C11" s="147"/>
       <c r="D11" s="20"/>
@@ -4119,7 +4137,7 @@
         <v>398929</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="89"/>
       <c r="C12" s="147"/>
       <c r="D12" s="20"/>
@@ -4128,7 +4146,7 @@
         <v>398929</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="89"/>
       <c r="C13" s="147"/>
       <c r="D13" s="22"/>
@@ -4137,7 +4155,7 @@
         <v>398929</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="89"/>
       <c r="C14" s="147"/>
       <c r="D14" s="20"/>
@@ -4146,7 +4164,7 @@
         <v>398929</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="89"/>
       <c r="C15" s="147"/>
       <c r="D15" s="20"/>
@@ -4155,7 +4173,7 @@
         <v>398929</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="89"/>
       <c r="C16" s="147"/>
       <c r="D16" s="20"/>
@@ -4164,7 +4182,7 @@
         <v>398929</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="89"/>
       <c r="C17" s="147"/>
       <c r="D17" s="20"/>
@@ -4173,7 +4191,7 @@
         <v>398929</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="89"/>
       <c r="C18" s="147"/>
       <c r="D18" s="20"/>
@@ -4182,301 +4200,301 @@
         <v>398929</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="30"/>
       <c r="C19" s="147"/>
       <c r="D19" s="138"/>
       <c r="E19" s="138"/>
     </row>
-    <row r="20" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="130"/>
       <c r="B20" s="110"/>
       <c r="C20" s="148"/>
       <c r="D20" s="60"/>
       <c r="E20" s="60"/>
     </row>
-    <row r="21" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="130"/>
       <c r="B21" s="110"/>
       <c r="C21" s="148"/>
       <c r="D21" s="60"/>
       <c r="E21" s="60"/>
     </row>
-    <row r="22" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="130"/>
       <c r="B22" s="110"/>
       <c r="C22" s="148"/>
       <c r="D22" s="60"/>
       <c r="E22" s="60"/>
     </row>
-    <row r="23" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="130"/>
       <c r="B23" s="110"/>
       <c r="C23" s="148"/>
       <c r="D23" s="60"/>
       <c r="E23" s="60"/>
     </row>
-    <row r="24" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="130"/>
       <c r="B24" s="110"/>
       <c r="C24" s="148"/>
       <c r="D24" s="60"/>
       <c r="E24" s="60"/>
     </row>
-    <row r="25" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="130"/>
       <c r="B25" s="110"/>
       <c r="C25" s="148"/>
       <c r="D25" s="60"/>
       <c r="E25" s="60"/>
     </row>
-    <row r="26" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="130"/>
       <c r="B26" s="110"/>
       <c r="C26" s="148"/>
       <c r="D26" s="60"/>
       <c r="E26" s="60"/>
     </row>
-    <row r="27" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="130"/>
       <c r="B27" s="110"/>
       <c r="C27" s="148"/>
       <c r="D27" s="60"/>
       <c r="E27" s="60"/>
     </row>
-    <row r="28" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="130"/>
       <c r="B28" s="110"/>
       <c r="C28" s="148"/>
       <c r="D28" s="60"/>
       <c r="E28" s="60"/>
     </row>
-    <row r="29" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="130"/>
       <c r="B29" s="110"/>
       <c r="C29" s="148"/>
       <c r="D29" s="60"/>
       <c r="E29" s="60"/>
     </row>
-    <row r="30" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="130"/>
       <c r="B30" s="110"/>
       <c r="C30" s="148"/>
       <c r="D30" s="60"/>
       <c r="E30" s="60"/>
     </row>
-    <row r="31" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="130"/>
       <c r="B31" s="110"/>
       <c r="C31" s="148"/>
       <c r="D31" s="60"/>
       <c r="E31" s="60"/>
     </row>
-    <row r="32" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="130"/>
       <c r="B32" s="110"/>
       <c r="C32" s="148"/>
       <c r="D32" s="60"/>
       <c r="E32" s="60"/>
     </row>
-    <row r="33" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="130"/>
       <c r="B33" s="110"/>
       <c r="C33" s="148"/>
       <c r="D33" s="60"/>
       <c r="E33" s="60"/>
     </row>
-    <row r="34" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="130"/>
       <c r="B34" s="110"/>
       <c r="C34" s="148"/>
       <c r="D34" s="60"/>
       <c r="E34" s="60"/>
     </row>
-    <row r="35" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="130"/>
       <c r="B35" s="110"/>
       <c r="C35" s="148"/>
       <c r="D35" s="60"/>
       <c r="E35" s="60"/>
     </row>
-    <row r="36" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="130"/>
       <c r="B36" s="110"/>
       <c r="C36" s="148"/>
       <c r="D36" s="60"/>
       <c r="E36" s="60"/>
     </row>
-    <row r="37" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="130"/>
       <c r="B37" s="110"/>
       <c r="C37" s="148"/>
       <c r="D37" s="60"/>
       <c r="E37" s="60"/>
     </row>
-    <row r="38" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="130"/>
       <c r="B38" s="110"/>
       <c r="C38" s="148"/>
       <c r="D38" s="60"/>
       <c r="E38" s="60"/>
     </row>
-    <row r="39" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="130"/>
       <c r="B39" s="110"/>
       <c r="C39" s="148"/>
       <c r="D39" s="60"/>
       <c r="E39" s="60"/>
     </row>
-    <row r="40" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="130"/>
       <c r="B40" s="110"/>
       <c r="C40" s="148"/>
       <c r="D40" s="60"/>
       <c r="E40" s="60"/>
     </row>
-    <row r="41" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="130"/>
       <c r="B41" s="110"/>
       <c r="C41" s="148"/>
       <c r="D41" s="60"/>
       <c r="E41" s="60"/>
     </row>
-    <row r="42" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="130"/>
       <c r="B42" s="110"/>
       <c r="C42" s="148"/>
       <c r="D42" s="60"/>
       <c r="E42" s="60"/>
     </row>
-    <row r="43" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="130"/>
       <c r="B43" s="110"/>
       <c r="C43" s="148"/>
       <c r="D43" s="60"/>
       <c r="E43" s="60"/>
     </row>
-    <row r="44" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="130"/>
       <c r="B44" s="110"/>
       <c r="C44" s="148"/>
       <c r="D44" s="60"/>
       <c r="E44" s="60"/>
     </row>
-    <row r="45" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="130"/>
       <c r="B45" s="110"/>
       <c r="C45" s="148"/>
       <c r="D45" s="143"/>
       <c r="E45" s="60"/>
     </row>
-    <row r="46" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="130"/>
       <c r="B46" s="110"/>
       <c r="C46" s="148"/>
       <c r="D46" s="60"/>
       <c r="E46" s="60"/>
     </row>
-    <row r="47" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="130"/>
       <c r="B47" s="110"/>
       <c r="C47" s="148"/>
       <c r="D47" s="60"/>
       <c r="E47" s="60"/>
     </row>
-    <row r="48" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="130"/>
       <c r="B48" s="110"/>
       <c r="C48" s="148"/>
       <c r="D48" s="60"/>
       <c r="E48" s="60"/>
     </row>
-    <row r="49" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="130"/>
       <c r="B49" s="110"/>
       <c r="C49" s="148"/>
       <c r="D49" s="60"/>
       <c r="E49" s="60"/>
     </row>
-    <row r="50" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="130"/>
       <c r="B50" s="110"/>
       <c r="C50" s="148"/>
       <c r="D50" s="60"/>
       <c r="E50" s="60"/>
     </row>
-    <row r="51" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="130"/>
       <c r="B51" s="110"/>
       <c r="C51" s="148"/>
       <c r="D51" s="60"/>
       <c r="E51" s="60"/>
     </row>
-    <row r="52" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="130"/>
       <c r="B52" s="110"/>
       <c r="C52" s="148"/>
       <c r="D52" s="60"/>
       <c r="E52" s="60"/>
     </row>
-    <row r="53" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="130"/>
       <c r="B53" s="110"/>
       <c r="C53" s="148"/>
       <c r="D53" s="62"/>
       <c r="E53" s="60"/>
     </row>
-    <row r="54" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="130"/>
       <c r="B54" s="110"/>
       <c r="C54" s="148"/>
       <c r="D54" s="60"/>
       <c r="E54" s="60"/>
     </row>
-    <row r="55" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="130"/>
       <c r="B55" s="110"/>
       <c r="C55" s="148"/>
       <c r="D55" s="60"/>
       <c r="E55" s="60"/>
     </row>
-    <row r="56" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" s="130"/>
       <c r="B56" s="110"/>
       <c r="C56" s="148"/>
       <c r="D56" s="60"/>
       <c r="E56" s="60"/>
     </row>
-    <row r="57" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="130"/>
       <c r="B57" s="110"/>
       <c r="C57" s="148"/>
       <c r="D57" s="60"/>
       <c r="E57" s="60"/>
     </row>
-    <row r="58" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" s="130"/>
       <c r="B58" s="110"/>
       <c r="C58" s="148"/>
       <c r="D58" s="60"/>
       <c r="E58" s="60"/>
     </row>
-    <row r="59" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="130"/>
       <c r="B59" s="110"/>
       <c r="C59" s="148"/>
       <c r="D59" s="60"/>
       <c r="E59" s="60"/>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D60" s="131"/>
       <c r="E60" s="60"/>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D61" s="131"/>
       <c r="E61" s="139"/>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D62" s="131"/>
       <c r="E62" s="130"/>
     </row>
@@ -4516,27 +4534,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="168" t="s">
+      <c r="A1" s="169" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="169"/>
-      <c r="C1" s="169"/>
-      <c r="D1" s="169"/>
-      <c r="E1" s="169"/>
-      <c r="F1" s="169"/>
-      <c r="G1" s="169"/>
+      <c r="B1" s="170"/>
+      <c r="C1" s="170"/>
+      <c r="D1" s="170"/>
+      <c r="E1" s="170"/>
+      <c r="F1" s="170"/>
+      <c r="G1" s="170"/>
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="170" t="s">
+      <c r="A2" s="171" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="170"/>
-      <c r="C2" s="170"/>
-      <c r="D2" s="170"/>
-      <c r="E2" s="170"/>
-      <c r="F2" s="170"/>
-      <c r="G2" s="170"/>
+      <c r="B2" s="171"/>
+      <c r="C2" s="171"/>
+      <c r="D2" s="171"/>
+      <c r="E2" s="171"/>
+      <c r="F2" s="171"/>
+      <c r="G2" s="171"/>
       <c r="H2" s="5"/>
       <c r="I2" s="2"/>
     </row>
@@ -4731,11 +4749,11 @@
         <v>161427</v>
       </c>
       <c r="F11" s="21"/>
-      <c r="G11" s="171">
+      <c r="G11" s="172">
         <f>SUM(H4:H10)</f>
         <v>48874</v>
       </c>
-      <c r="H11" s="172"/>
+      <c r="H11" s="173"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="12"/>
@@ -6110,11 +6128,11 @@
         <v>76469.81</v>
       </c>
       <c r="F81" s="61"/>
-      <c r="G81" s="173">
+      <c r="G81" s="174">
         <f>SUM(H67:H80)</f>
         <v>76469.81</v>
       </c>
-      <c r="H81" s="174"/>
+      <c r="H81" s="175"/>
     </row>
     <row r="82" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="23"/>
@@ -6202,12 +6220,12 @@
       <c r="B88" s="37"/>
       <c r="C88" s="38"/>
       <c r="D88" s="2"/>
-      <c r="E88" s="154">
+      <c r="E88" s="155">
         <f>E84-G84</f>
         <v>1332859.9100000001</v>
       </c>
-      <c r="F88" s="155"/>
-      <c r="G88" s="156"/>
+      <c r="F88" s="156"/>
+      <c r="G88" s="157"/>
       <c r="H88" s="44"/>
       <c r="I88" s="2"/>
     </row>
@@ -6224,11 +6242,11 @@
       <c r="B90" s="37"/>
       <c r="C90" s="38"/>
       <c r="D90" s="2"/>
-      <c r="E90" s="157" t="s">
+      <c r="E90" s="158" t="s">
         <v>8</v>
       </c>
-      <c r="F90" s="157"/>
-      <c r="G90" s="157"/>
+      <c r="F90" s="158"/>
+      <c r="G90" s="158"/>
       <c r="I90" s="2"/>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
@@ -6373,25 +6391,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="158" t="s">
+      <c r="B1" s="159" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="159"/>
-      <c r="D1" s="159"/>
-      <c r="E1" s="159"/>
-      <c r="F1" s="159"/>
-      <c r="G1" s="160"/>
+      <c r="C1" s="160"/>
+      <c r="D1" s="160"/>
+      <c r="E1" s="160"/>
+      <c r="F1" s="160"/>
+      <c r="G1" s="161"/>
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
-      <c r="B2" s="153" t="s">
+      <c r="B2" s="154" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="153"/>
-      <c r="D2" s="153"/>
-      <c r="E2" s="153"/>
-      <c r="F2" s="153"/>
+      <c r="C2" s="154"/>
+      <c r="D2" s="154"/>
+      <c r="E2" s="154"/>
+      <c r="F2" s="154"/>
       <c r="G2" s="4"/>
       <c r="H2" s="5"/>
       <c r="I2" s="2"/>
@@ -7283,12 +7301,12 @@
       <c r="B52" s="37"/>
       <c r="C52" s="38"/>
       <c r="D52" s="2"/>
-      <c r="E52" s="154">
+      <c r="E52" s="155">
         <f>E48-G48</f>
         <v>734621</v>
       </c>
-      <c r="F52" s="155"/>
-      <c r="G52" s="156"/>
+      <c r="F52" s="156"/>
+      <c r="G52" s="157"/>
       <c r="I52" s="2"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
@@ -7304,11 +7322,11 @@
       <c r="B54" s="37"/>
       <c r="C54" s="38"/>
       <c r="D54" s="2"/>
-      <c r="E54" s="157" t="s">
+      <c r="E54" s="158" t="s">
         <v>8</v>
       </c>
-      <c r="F54" s="157"/>
-      <c r="G54" s="157"/>
+      <c r="F54" s="158"/>
+      <c r="G54" s="158"/>
       <c r="I54" s="2"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
@@ -7464,25 +7482,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="158" t="s">
+      <c r="B1" s="159" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="159"/>
-      <c r="D1" s="159"/>
-      <c r="E1" s="159"/>
-      <c r="F1" s="159"/>
-      <c r="G1" s="160"/>
+      <c r="C1" s="160"/>
+      <c r="D1" s="160"/>
+      <c r="E1" s="160"/>
+      <c r="F1" s="160"/>
+      <c r="G1" s="161"/>
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
-      <c r="B2" s="153" t="s">
+      <c r="B2" s="154" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="153"/>
-      <c r="D2" s="153"/>
-      <c r="E2" s="153"/>
-      <c r="F2" s="153"/>
+      <c r="C2" s="154"/>
+      <c r="D2" s="154"/>
+      <c r="E2" s="154"/>
+      <c r="F2" s="154"/>
       <c r="G2" s="4"/>
       <c r="H2" s="5"/>
       <c r="I2" s="2"/>
@@ -9212,12 +9230,12 @@
       <c r="B76" s="37"/>
       <c r="C76" s="38"/>
       <c r="D76" s="2"/>
-      <c r="E76" s="154">
+      <c r="E76" s="155">
         <f>E72-G72</f>
         <v>0</v>
       </c>
-      <c r="F76" s="155"/>
-      <c r="G76" s="156"/>
+      <c r="F76" s="156"/>
+      <c r="G76" s="157"/>
       <c r="I76" s="2"/>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
@@ -9233,11 +9251,11 @@
       <c r="B78" s="37"/>
       <c r="C78" s="38"/>
       <c r="D78" s="2"/>
-      <c r="E78" s="157" t="s">
+      <c r="E78" s="158" t="s">
         <v>8</v>
       </c>
-      <c r="F78" s="157"/>
-      <c r="G78" s="157"/>
+      <c r="F78" s="158"/>
+      <c r="G78" s="158"/>
       <c r="I78" s="2"/>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
@@ -9378,25 +9396,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="158" t="s">
+      <c r="B1" s="159" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="159"/>
-      <c r="D1" s="159"/>
-      <c r="E1" s="159"/>
-      <c r="F1" s="159"/>
-      <c r="G1" s="160"/>
+      <c r="C1" s="160"/>
+      <c r="D1" s="160"/>
+      <c r="E1" s="160"/>
+      <c r="F1" s="160"/>
+      <c r="G1" s="161"/>
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
-      <c r="B2" s="153" t="s">
+      <c r="B2" s="154" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="153"/>
-      <c r="D2" s="153"/>
-      <c r="E2" s="153"/>
-      <c r="F2" s="153"/>
+      <c r="C2" s="154"/>
+      <c r="D2" s="154"/>
+      <c r="E2" s="154"/>
+      <c r="F2" s="154"/>
       <c r="G2" s="4"/>
       <c r="H2" s="5"/>
       <c r="I2" s="2"/>
@@ -10245,12 +10263,12 @@
       <c r="B41" s="37"/>
       <c r="C41" s="38"/>
       <c r="D41" s="2"/>
-      <c r="E41" s="154">
+      <c r="E41" s="155">
         <f>E37-G37</f>
         <v>0</v>
       </c>
-      <c r="F41" s="155"/>
-      <c r="G41" s="156"/>
+      <c r="F41" s="156"/>
+      <c r="G41" s="157"/>
       <c r="I41" s="2"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -10266,11 +10284,11 @@
       <c r="B43" s="37"/>
       <c r="C43" s="38"/>
       <c r="D43" s="2"/>
-      <c r="E43" s="157" t="s">
+      <c r="E43" s="158" t="s">
         <v>8</v>
       </c>
-      <c r="F43" s="157"/>
-      <c r="G43" s="157"/>
+      <c r="F43" s="158"/>
+      <c r="G43" s="158"/>
       <c r="I43" s="2"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
@@ -10414,25 +10432,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="161" t="s">
+      <c r="B1" s="162" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="162"/>
-      <c r="D1" s="162"/>
-      <c r="E1" s="162"/>
-      <c r="F1" s="162"/>
-      <c r="G1" s="163"/>
+      <c r="C1" s="163"/>
+      <c r="D1" s="163"/>
+      <c r="E1" s="163"/>
+      <c r="F1" s="163"/>
+      <c r="G1" s="164"/>
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
-      <c r="B2" s="153" t="s">
+      <c r="B2" s="154" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="153"/>
-      <c r="D2" s="153"/>
-      <c r="E2" s="153"/>
-      <c r="F2" s="153"/>
+      <c r="C2" s="154"/>
+      <c r="D2" s="154"/>
+      <c r="E2" s="154"/>
+      <c r="F2" s="154"/>
       <c r="G2" s="4"/>
       <c r="H2" s="5"/>
       <c r="I2" s="2"/>
@@ -11772,12 +11790,12 @@
       <c r="B60" s="37"/>
       <c r="C60" s="38"/>
       <c r="D60" s="2"/>
-      <c r="E60" s="154">
+      <c r="E60" s="155">
         <f>E56-G56</f>
         <v>0</v>
       </c>
-      <c r="F60" s="155"/>
-      <c r="G60" s="156"/>
+      <c r="F60" s="156"/>
+      <c r="G60" s="157"/>
       <c r="I60" s="2"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
@@ -11793,11 +11811,11 @@
       <c r="B62" s="37"/>
       <c r="C62" s="38"/>
       <c r="D62" s="2"/>
-      <c r="E62" s="157" t="s">
+      <c r="E62" s="158" t="s">
         <v>8</v>
       </c>
-      <c r="F62" s="157"/>
-      <c r="G62" s="157"/>
+      <c r="F62" s="158"/>
+      <c r="G62" s="158"/>
       <c r="I62" s="2"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
@@ -11938,25 +11956,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="161" t="s">
+      <c r="B1" s="162" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="162"/>
-      <c r="D1" s="162"/>
-      <c r="E1" s="162"/>
-      <c r="F1" s="162"/>
-      <c r="G1" s="163"/>
+      <c r="C1" s="163"/>
+      <c r="D1" s="163"/>
+      <c r="E1" s="163"/>
+      <c r="F1" s="163"/>
+      <c r="G1" s="164"/>
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
-      <c r="B2" s="153" t="s">
+      <c r="B2" s="154" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="153"/>
-      <c r="D2" s="153"/>
-      <c r="E2" s="153"/>
-      <c r="F2" s="153"/>
+      <c r="C2" s="154"/>
+      <c r="D2" s="154"/>
+      <c r="E2" s="154"/>
+      <c r="F2" s="154"/>
       <c r="G2" s="4"/>
       <c r="H2" s="5"/>
       <c r="I2" s="2"/>
@@ -13357,12 +13375,12 @@
       <c r="B61" s="37"/>
       <c r="C61" s="38"/>
       <c r="D61" s="2"/>
-      <c r="E61" s="154">
+      <c r="E61" s="155">
         <f>E57-G57</f>
         <v>0</v>
       </c>
-      <c r="F61" s="155"/>
-      <c r="G61" s="156"/>
+      <c r="F61" s="156"/>
+      <c r="G61" s="157"/>
       <c r="I61" s="2"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
@@ -13378,11 +13396,11 @@
       <c r="B63" s="37"/>
       <c r="C63" s="38"/>
       <c r="D63" s="2"/>
-      <c r="E63" s="157" t="s">
+      <c r="E63" s="158" t="s">
         <v>8</v>
       </c>
-      <c r="F63" s="157"/>
-      <c r="G63" s="157"/>
+      <c r="F63" s="158"/>
+      <c r="G63" s="158"/>
       <c r="I63" s="2"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
@@ -13523,25 +13541,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="161" t="s">
+      <c r="B1" s="162" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="162"/>
-      <c r="D1" s="162"/>
-      <c r="E1" s="162"/>
-      <c r="F1" s="162"/>
-      <c r="G1" s="163"/>
+      <c r="C1" s="163"/>
+      <c r="D1" s="163"/>
+      <c r="E1" s="163"/>
+      <c r="F1" s="163"/>
+      <c r="G1" s="164"/>
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
-      <c r="B2" s="153" t="s">
+      <c r="B2" s="154" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="153"/>
-      <c r="D2" s="153"/>
-      <c r="E2" s="153"/>
-      <c r="F2" s="153"/>
+      <c r="C2" s="154"/>
+      <c r="D2" s="154"/>
+      <c r="E2" s="154"/>
+      <c r="F2" s="154"/>
       <c r="G2" s="4"/>
       <c r="H2" s="5"/>
       <c r="I2" s="2"/>
@@ -14991,12 +15009,12 @@
       <c r="B64" s="37"/>
       <c r="C64" s="38"/>
       <c r="D64" s="2"/>
-      <c r="E64" s="154">
+      <c r="E64" s="155">
         <f>E60-G60</f>
         <v>0</v>
       </c>
-      <c r="F64" s="155"/>
-      <c r="G64" s="156"/>
+      <c r="F64" s="156"/>
+      <c r="G64" s="157"/>
       <c r="I64" s="2"/>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
@@ -15012,11 +15030,11 @@
       <c r="B66" s="37"/>
       <c r="C66" s="38"/>
       <c r="D66" s="2"/>
-      <c r="E66" s="157" t="s">
+      <c r="E66" s="158" t="s">
         <v>8</v>
       </c>
-      <c r="F66" s="157"/>
-      <c r="G66" s="157"/>
+      <c r="F66" s="158"/>
+      <c r="G66" s="158"/>
       <c r="I66" s="2"/>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
@@ -15139,8 +15157,8 @@
   </sheetPr>
   <dimension ref="A1:I80"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="F52" sqref="F52"/>
+    <sheetView topLeftCell="B39" workbookViewId="0">
+      <selection activeCell="I44" sqref="I44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -15157,25 +15175,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="161" t="s">
+      <c r="B1" s="162" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="162"/>
-      <c r="D1" s="162"/>
-      <c r="E1" s="162"/>
-      <c r="F1" s="162"/>
-      <c r="G1" s="163"/>
+      <c r="C1" s="163"/>
+      <c r="D1" s="163"/>
+      <c r="E1" s="163"/>
+      <c r="F1" s="163"/>
+      <c r="G1" s="164"/>
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
-      <c r="B2" s="153" t="s">
+      <c r="B2" s="154" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="153"/>
-      <c r="D2" s="153"/>
-      <c r="E2" s="153"/>
-      <c r="F2" s="153"/>
+      <c r="C2" s="154"/>
+      <c r="D2" s="154"/>
+      <c r="E2" s="154"/>
+      <c r="F2" s="154"/>
       <c r="G2" s="4"/>
       <c r="H2" s="5"/>
       <c r="I2" s="2"/>
@@ -16156,11 +16174,15 @@
       <c r="E43" s="20">
         <v>45974</v>
       </c>
-      <c r="F43" s="93"/>
-      <c r="G43" s="94"/>
+      <c r="F43" s="93">
+        <v>44692</v>
+      </c>
+      <c r="G43" s="94">
+        <v>45974</v>
+      </c>
       <c r="H43" s="18">
         <f t="shared" si="0"/>
-        <v>45974</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -16522,11 +16544,11 @@
       <c r="F61" s="39"/>
       <c r="G61" s="39">
         <f>SUM(G4:G60)</f>
-        <v>656494</v>
+        <v>702468</v>
       </c>
       <c r="H61" s="40">
         <f>SUM(H4:H60)</f>
-        <v>281628</v>
+        <v>235654</v>
       </c>
       <c r="I61" s="2"/>
     </row>
@@ -16568,12 +16590,12 @@
       <c r="B65" s="37"/>
       <c r="C65" s="38"/>
       <c r="D65" s="2"/>
-      <c r="E65" s="154">
+      <c r="E65" s="155">
         <f>E61-G61</f>
-        <v>281628</v>
-      </c>
-      <c r="F65" s="155"/>
-      <c r="G65" s="156"/>
+        <v>235654</v>
+      </c>
+      <c r="F65" s="156"/>
+      <c r="G65" s="157"/>
       <c r="I65" s="2"/>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
@@ -16589,11 +16611,11 @@
       <c r="B67" s="37"/>
       <c r="C67" s="38"/>
       <c r="D67" s="2"/>
-      <c r="E67" s="157" t="s">
+      <c r="E67" s="158" t="s">
         <v>8</v>
       </c>
-      <c r="F67" s="157"/>
-      <c r="G67" s="157"/>
+      <c r="F67" s="158"/>
+      <c r="G67" s="158"/>
       <c r="I67" s="2"/>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
@@ -16757,8 +16779,8 @@
   </sheetPr>
   <dimension ref="A1:I80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -16775,25 +16797,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="161" t="s">
+      <c r="B1" s="162" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="162"/>
-      <c r="D1" s="162"/>
-      <c r="E1" s="162"/>
-      <c r="F1" s="162"/>
-      <c r="G1" s="163"/>
+      <c r="C1" s="163"/>
+      <c r="D1" s="163"/>
+      <c r="E1" s="163"/>
+      <c r="F1" s="163"/>
+      <c r="G1" s="164"/>
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
-      <c r="B2" s="153" t="s">
+      <c r="B2" s="154" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="153"/>
-      <c r="D2" s="153"/>
-      <c r="E2" s="153"/>
-      <c r="F2" s="153"/>
+      <c r="C2" s="154"/>
+      <c r="D2" s="154"/>
+      <c r="E2" s="154"/>
+      <c r="F2" s="154"/>
       <c r="G2" s="4"/>
       <c r="H2" s="5"/>
       <c r="I2" s="2"/>
@@ -16880,11 +16902,15 @@
       <c r="E6" s="20">
         <v>1625</v>
       </c>
-      <c r="F6" s="21"/>
-      <c r="G6" s="22"/>
+      <c r="F6" s="21">
+        <v>44692</v>
+      </c>
+      <c r="G6" s="22">
+        <v>1625</v>
+      </c>
       <c r="H6" s="18">
         <f t="shared" si="0"/>
-        <v>1625</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -16993,63 +17019,87 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="12"/>
+      <c r="A12" s="12">
+        <v>44687</v>
+      </c>
       <c r="B12" s="13">
         <v>348</v>
       </c>
       <c r="C12" s="24"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="20"/>
+      <c r="D12" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12" s="20">
+        <v>10275</v>
+      </c>
       <c r="F12" s="21"/>
       <c r="G12" s="22"/>
       <c r="H12" s="18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>10275</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="12"/>
+      <c r="A13" s="12">
+        <v>44690</v>
+      </c>
       <c r="B13" s="13">
         <v>349</v>
       </c>
       <c r="C13" s="25"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="20"/>
+      <c r="D13" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="E13" s="20">
+        <v>12858</v>
+      </c>
       <c r="F13" s="21"/>
       <c r="G13" s="22"/>
       <c r="H13" s="18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>12858</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="12"/>
+      <c r="A14" s="12">
+        <v>44691</v>
+      </c>
       <c r="B14" s="13">
         <v>350</v>
       </c>
       <c r="C14" s="24"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="20"/>
+      <c r="D14" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" s="20">
+        <v>23765</v>
+      </c>
       <c r="F14" s="21"/>
       <c r="G14" s="22"/>
       <c r="H14" s="18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>23765</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="12"/>
+      <c r="A15" s="12">
+        <v>44692</v>
+      </c>
       <c r="B15" s="13">
         <v>351</v>
       </c>
       <c r="C15" s="25"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="20"/>
+      <c r="D15" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="E15" s="20">
+        <v>1560</v>
+      </c>
       <c r="F15" s="21"/>
       <c r="G15" s="22"/>
       <c r="H15" s="18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1560</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -17731,16 +17781,16 @@
       <c r="D61" s="2"/>
       <c r="E61" s="39">
         <f>SUM(E4:E60)</f>
-        <v>258291</v>
+        <v>306749</v>
       </c>
       <c r="F61" s="39"/>
       <c r="G61" s="39">
         <f>SUM(G4:G60)</f>
-        <v>0</v>
+        <v>1625</v>
       </c>
       <c r="H61" s="40">
         <f>SUM(H4:H60)</f>
-        <v>258291</v>
+        <v>305124</v>
       </c>
       <c r="I61" s="2"/>
     </row>
@@ -17782,12 +17832,12 @@
       <c r="B65" s="37"/>
       <c r="C65" s="38"/>
       <c r="D65" s="2"/>
-      <c r="E65" s="154">
+      <c r="E65" s="155">
         <f>E61-G61</f>
-        <v>258291</v>
-      </c>
-      <c r="F65" s="155"/>
-      <c r="G65" s="156"/>
+        <v>305124</v>
+      </c>
+      <c r="F65" s="156"/>
+      <c r="G65" s="157"/>
       <c r="I65" s="2"/>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
@@ -17803,11 +17853,11 @@
       <c r="B67" s="37"/>
       <c r="C67" s="38"/>
       <c r="D67" s="2"/>
-      <c r="E67" s="157" t="s">
+      <c r="E67" s="158" t="s">
         <v>8</v>
       </c>
-      <c r="F67" s="157"/>
-      <c r="G67" s="157"/>
+      <c r="F67" s="158"/>
+      <c r="G67" s="158"/>
       <c r="I67" s="2"/>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
CIERRE 25 MAYO 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #05  MAYO  2022/CREDITOS  4 CARNES   ZAVALETA   MAYO    2022.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #05  MAYO  2022/CREDITOS  4 CARNES   ZAVALETA   MAYO    2022.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6015" yWindow="330" windowWidth="13905" windowHeight="10920" firstSheet="7" activeTab="7"/>
+    <workbookView xWindow="6015" yWindow="330" windowWidth="13905" windowHeight="10920" firstSheet="8" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="REMISIONES OCTUBRE  2021     " sheetId="4" r:id="rId1"/>
@@ -3999,10 +3999,10 @@
   <sheetPr>
     <tabColor rgb="FFC00000"/>
   </sheetPr>
-  <dimension ref="A1:F62"/>
+  <dimension ref="A1:H62"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -4015,14 +4015,14 @@
     <col min="7" max="16384" width="11.42578125" style="123"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="165"/>
       <c r="B1" s="166"/>
       <c r="C1" s="166"/>
       <c r="D1" s="166"/>
       <c r="E1" s="166"/>
     </row>
-    <row r="2" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:8" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="167" t="s">
         <v>43</v>
       </c>
@@ -4031,7 +4031,7 @@
       <c r="D2" s="168"/>
       <c r="E2" s="168"/>
     </row>
-    <row r="3" spans="1:6" ht="33.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:8" ht="33.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="142" t="s">
         <v>44</v>
       </c>
@@ -4045,7 +4045,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="140">
         <v>44690</v>
       </c>
@@ -4063,7 +4063,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="89">
         <v>44691</v>
       </c>
@@ -4078,7 +4078,7 @@
         <v>142189</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="89">
         <v>44692</v>
       </c>
@@ -4093,7 +4093,7 @@
         <v>207018</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="89">
         <v>44693</v>
       </c>
@@ -4108,7 +4108,7 @@
         <v>247093</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="89">
         <v>44694</v>
       </c>
@@ -4123,7 +4123,7 @@
         <v>303144</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="89">
         <v>44695</v>
       </c>
@@ -4137,8 +4137,11 @@
         <f t="shared" si="0"/>
         <v>346594</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H9" s="123">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="89">
         <v>44696</v>
       </c>
@@ -4153,67 +4156,109 @@
         <v>398929</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="89"/>
-      <c r="C11" s="147"/>
-      <c r="D11" s="20"/>
+    <row r="11" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="89">
+        <v>44697</v>
+      </c>
+      <c r="C11" s="147">
+        <v>44701</v>
+      </c>
+      <c r="D11" s="20">
+        <v>69191</v>
+      </c>
       <c r="E11" s="20">
         <f t="shared" si="0"/>
-        <v>398929</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="89"/>
-      <c r="C12" s="147"/>
-      <c r="D12" s="20"/>
+        <v>468120</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="89">
+        <v>44698</v>
+      </c>
+      <c r="C12" s="147">
+        <v>44701</v>
+      </c>
+      <c r="D12" s="20">
+        <v>50155</v>
+      </c>
       <c r="E12" s="20">
         <f t="shared" si="0"/>
-        <v>398929</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="89"/>
-      <c r="C13" s="147"/>
-      <c r="D13" s="22"/>
+        <v>518275</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="89">
+        <v>44699</v>
+      </c>
+      <c r="C13" s="147">
+        <v>44701</v>
+      </c>
+      <c r="D13" s="22">
+        <v>55227</v>
+      </c>
       <c r="E13" s="20">
         <f t="shared" si="0"/>
-        <v>398929</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="89"/>
-      <c r="C14" s="147"/>
-      <c r="D14" s="20"/>
+        <v>573502</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="89">
+        <v>44700</v>
+      </c>
+      <c r="C14" s="147">
+        <v>44701</v>
+      </c>
+      <c r="D14" s="20">
+        <v>47102</v>
+      </c>
       <c r="E14" s="20">
         <f t="shared" si="0"/>
-        <v>398929</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="89"/>
-      <c r="C15" s="147"/>
-      <c r="D15" s="20"/>
+        <v>620604</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="89">
+        <v>44701</v>
+      </c>
+      <c r="C15" s="147">
+        <v>44704</v>
+      </c>
+      <c r="D15" s="20">
+        <v>93134</v>
+      </c>
       <c r="E15" s="20">
         <f t="shared" si="0"/>
-        <v>398929</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="89"/>
-      <c r="C16" s="147"/>
-      <c r="D16" s="20"/>
+        <v>713738</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="89">
+        <v>44702</v>
+      </c>
+      <c r="C16" s="147">
+        <v>44704</v>
+      </c>
+      <c r="D16" s="20">
+        <v>22308</v>
+      </c>
       <c r="E16" s="20">
         <f t="shared" si="0"/>
-        <v>398929</v>
+        <v>736046</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="89"/>
-      <c r="C17" s="147"/>
-      <c r="D17" s="20"/>
+      <c r="B17" s="89">
+        <v>44703</v>
+      </c>
+      <c r="C17" s="147">
+        <v>44704</v>
+      </c>
+      <c r="D17" s="20">
+        <v>23536</v>
+      </c>
       <c r="E17" s="20">
         <f t="shared" si="0"/>
-        <v>398929</v>
+        <v>759582</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -4222,7 +4267,7 @@
       <c r="D18" s="20"/>
       <c r="E18" s="20">
         <f t="shared" si="0"/>
-        <v>398929</v>
+        <v>759582</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -16808,7 +16853,7 @@
   </sheetPr>
   <dimension ref="A1:I80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
CIERRE 26 MAY 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #05  MAYO  2022/CREDITOS  4 CARNES   ZAVALETA   MAYO    2022.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #05  MAYO  2022/CREDITOS  4 CARNES   ZAVALETA   MAYO    2022.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6015" yWindow="330" windowWidth="13905" windowHeight="10920" firstSheet="8" activeTab="9"/>
+    <workbookView xWindow="6015" yWindow="330" windowWidth="13905" windowHeight="10920" firstSheet="7" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="REMISIONES OCTUBRE  2021     " sheetId="4" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="88">
   <si>
     <t>REMISION</t>
   </si>
@@ -332,6 +332,108 @@
   <si>
     <t>GRACIELA LEDO PARRA</t>
   </si>
+  <si>
+    <t>09/04/2022</t>
+  </si>
+  <si>
+    <t>C-18193</t>
+  </si>
+  <si>
+    <t>C-18265</t>
+  </si>
+  <si>
+    <t>11/04/2022</t>
+  </si>
+  <si>
+    <t>C-18374</t>
+  </si>
+  <si>
+    <t>C-18375</t>
+  </si>
+  <si>
+    <t>12/04/2022</t>
+  </si>
+  <si>
+    <t>C-18521</t>
+  </si>
+  <si>
+    <t>13/04/2022</t>
+  </si>
+  <si>
+    <t>C-18625</t>
+  </si>
+  <si>
+    <t>14/04/2022</t>
+  </si>
+  <si>
+    <t>C-18733</t>
+  </si>
+  <si>
+    <t>C-18776</t>
+  </si>
+  <si>
+    <t>16/04/2022</t>
+  </si>
+  <si>
+    <t>C-18883</t>
+  </si>
+  <si>
+    <t>18/04/2022</t>
+  </si>
+  <si>
+    <t>C-19081</t>
+  </si>
+  <si>
+    <t>19/04/2022</t>
+  </si>
+  <si>
+    <t>C-19160</t>
+  </si>
+  <si>
+    <t>C-19170</t>
+  </si>
+  <si>
+    <t>C-19216</t>
+  </si>
+  <si>
+    <t>20/04/2022</t>
+  </si>
+  <si>
+    <t>C-19283</t>
+  </si>
+  <si>
+    <t>C-19315</t>
+  </si>
+  <si>
+    <t>21/04/2022</t>
+  </si>
+  <si>
+    <t>C-19425</t>
+  </si>
+  <si>
+    <t>22/04/2022</t>
+  </si>
+  <si>
+    <t>C-19561</t>
+  </si>
+  <si>
+    <t>C-19605</t>
+  </si>
+  <si>
+    <t>23/04/2022</t>
+  </si>
+  <si>
+    <t>C-19642</t>
+  </si>
+  <si>
+    <t>C-19644</t>
+  </si>
+  <si>
+    <t>C-19690</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEPOSITOS APLICADOS </t>
+  </si>
 </sst>
 </file>
 
@@ -536,7 +638,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -612,6 +714,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00FF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF99CCFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -884,7 +992,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="176">
+  <cellXfs count="188">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1173,7 +1281,6 @@
     <xf numFmtId="165" fontId="10" fillId="9" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1211,6 +1318,29 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="7" fillId="14" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="7" fillId="14" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="3" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="2" fillId="9" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="9" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="9" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="15" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="22" fillId="13" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1286,11 +1416,11 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF00FF00"/>
       <color rgb="FFCC0099"/>
       <color rgb="FF0000FF"/>
       <color rgb="FFCC99FF"/>
       <color rgb="FF990033"/>
-      <color rgb="FF00FF00"/>
       <color rgb="FF66FFFF"/>
       <color rgb="FF9966FF"/>
       <color rgb="FFFF9900"/>
@@ -1419,6 +1549,117 @@
 </file>
 
 <file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>647703</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>152402</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>180974</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>133349</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="2" name="1 Conector recto de flecha">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="4576765" y="27922540"/>
+          <a:ext cx="581022" cy="590546"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>561977</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>123829</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>161927</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="2 Conector recto de flecha">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="5472114" y="27970167"/>
+          <a:ext cx="638173" cy="495298"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing11.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -2311,101 +2552,44 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>647703</xdr:colOff>
-      <xdr:row>84</xdr:row>
-      <xdr:rowOff>152402</xdr:rowOff>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>180974</xdr:colOff>
-      <xdr:row>86</xdr:row>
-      <xdr:rowOff>133349</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="2" name="1 Conector recto de flecha">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="5" name="Conector angular 4"/>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm rot="16200000" flipH="1">
-          <a:off x="4576765" y="27922540"/>
-          <a:ext cx="581022" cy="590546"/>
+        <a:xfrm>
+          <a:off x="3848100" y="5753100"/>
+          <a:ext cx="4619625" cy="1123950"/>
         </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 30000"/>
+          </a:avLst>
         </a:prstGeom>
         <a:ln>
-          <a:tailEnd type="arrow"/>
+          <a:tailEnd type="triangle"/>
         </a:ln>
       </xdr:spPr>
       <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="dk1"/>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent2"/>
         </a:lnRef>
         <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
+          <a:schemeClr val="accent2"/>
         </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>561977</xdr:colOff>
-      <xdr:row>84</xdr:row>
-      <xdr:rowOff>123829</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>86</xdr:row>
-      <xdr:rowOff>161927</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="3" name="2 Conector recto de flecha">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000003000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="5400000">
-          <a:off x="5472114" y="27970167"/>
-          <a:ext cx="638173" cy="495298"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="arrow"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="dk1"/>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent2"/>
         </a:effectRef>
         <a:fontRef idx="minor">
           <a:schemeClr val="tx1"/>
@@ -2704,24 +2888,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="159" t="s">
+      <c r="B1" s="171" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="160"/>
-      <c r="D1" s="160"/>
-      <c r="E1" s="160"/>
-      <c r="F1" s="161"/>
+      <c r="C1" s="172"/>
+      <c r="D1" s="172"/>
+      <c r="E1" s="172"/>
+      <c r="F1" s="173"/>
       <c r="H1" s="2"/>
     </row>
     <row r="2" spans="1:8" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
-      <c r="B2" s="154" t="s">
+      <c r="B2" s="166" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="154"/>
-      <c r="D2" s="154"/>
-      <c r="E2" s="154"/>
-      <c r="F2" s="154"/>
+      <c r="C2" s="166"/>
+      <c r="D2" s="166"/>
+      <c r="E2" s="166"/>
+      <c r="F2" s="166"/>
       <c r="G2" s="5"/>
       <c r="H2" s="2"/>
     </row>
@@ -3867,12 +4051,12 @@
     <row r="55" spans="1:8" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B55" s="37"/>
       <c r="C55" s="2"/>
-      <c r="D55" s="155">
+      <c r="D55" s="167">
         <f>D51-F51</f>
         <v>0</v>
       </c>
-      <c r="E55" s="156"/>
-      <c r="F55" s="157"/>
+      <c r="E55" s="168"/>
+      <c r="F55" s="169"/>
       <c r="H55" s="2"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
@@ -3886,11 +4070,11 @@
     <row r="57" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B57" s="37"/>
       <c r="C57" s="2"/>
-      <c r="D57" s="158" t="s">
+      <c r="D57" s="170" t="s">
         <v>8</v>
       </c>
-      <c r="E57" s="158"/>
-      <c r="F57" s="158"/>
+      <c r="E57" s="170"/>
+      <c r="F57" s="170"/>
       <c r="H57" s="2"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
@@ -3999,75 +4183,124 @@
   <sheetPr>
     <tabColor rgb="FFC00000"/>
   </sheetPr>
-  <dimension ref="A1:H62"/>
+  <dimension ref="A1:K62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="11.42578125" style="123"/>
-    <col min="3" max="3" width="14.85546875" style="149" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" style="148" customWidth="1"/>
     <col min="4" max="4" width="16.7109375" style="124" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" style="123" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" style="153"/>
-    <col min="7" max="16384" width="11.42578125" style="123"/>
+    <col min="5" max="5" width="15.5703125" style="123" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" style="152"/>
+    <col min="7" max="8" width="11.42578125" style="123"/>
+    <col min="9" max="9" width="13.85546875" style="123" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" style="123"/>
+    <col min="11" max="11" width="17.42578125" style="123" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="11.42578125" style="123"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="165"/>
-      <c r="B1" s="166"/>
-      <c r="C1" s="166"/>
-      <c r="D1" s="166"/>
-      <c r="E1" s="166"/>
-    </row>
-    <row r="2" spans="1:8" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="167" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="177"/>
+      <c r="B1" s="178"/>
+      <c r="C1" s="178"/>
+      <c r="D1" s="178"/>
+      <c r="E1" s="178"/>
+    </row>
+    <row r="2" spans="1:11" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="179" t="s">
         <v>43</v>
       </c>
-      <c r="B2" s="168"/>
-      <c r="C2" s="168"/>
-      <c r="D2" s="168"/>
-      <c r="E2" s="168"/>
-    </row>
-    <row r="3" spans="1:8" ht="33.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="142" t="s">
+      <c r="B2" s="180"/>
+      <c r="C2" s="180"/>
+      <c r="D2" s="180"/>
+      <c r="E2" s="180"/>
+      <c r="G2" s="153" t="s">
+        <v>54</v>
+      </c>
+      <c r="H2" s="154" t="s">
+        <v>55</v>
+      </c>
+      <c r="I2" s="155">
+        <v>67001.67</v>
+      </c>
+      <c r="J2" s="156">
+        <v>44706</v>
+      </c>
+      <c r="K2" s="155">
+        <v>67001.67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="33.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B3" s="141" t="s">
         <v>44</v>
       </c>
-      <c r="C3" s="145" t="s">
+      <c r="C3" s="144" t="s">
         <v>45</v>
       </c>
-      <c r="D3" s="150" t="s">
+      <c r="D3" s="149" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="144" t="s">
+      <c r="E3" s="143" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="140">
+      <c r="G3" s="153" t="s">
+        <v>54</v>
+      </c>
+      <c r="H3" s="154" t="s">
+        <v>56</v>
+      </c>
+      <c r="I3" s="155">
+        <v>5256</v>
+      </c>
+      <c r="J3" s="156">
+        <v>44706</v>
+      </c>
+      <c r="K3" s="155">
+        <v>5256</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="139">
         <v>44690</v>
       </c>
-      <c r="C4" s="146">
+      <c r="C4" s="145">
         <v>44693</v>
       </c>
-      <c r="D4" s="141">
+      <c r="D4" s="140">
         <v>67500</v>
       </c>
-      <c r="E4" s="141">
+      <c r="E4" s="140">
         <f>D4</f>
         <v>67500</v>
       </c>
-      <c r="F4" s="153" t="s">
+      <c r="F4" s="152" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G4" s="153" t="s">
+        <v>57</v>
+      </c>
+      <c r="H4" s="154" t="s">
+        <v>58</v>
+      </c>
+      <c r="I4" s="155">
+        <v>40472.6</v>
+      </c>
+      <c r="J4" s="156">
+        <v>44706</v>
+      </c>
+      <c r="K4" s="155">
+        <v>40472.6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="89">
         <v>44691</v>
       </c>
-      <c r="C5" s="147">
+      <c r="C5" s="146">
         <v>44693</v>
       </c>
       <c r="D5" s="20">
@@ -4077,12 +4310,27 @@
         <f>E4+D5</f>
         <v>142189</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G5" s="153" t="s">
+        <v>57</v>
+      </c>
+      <c r="H5" s="154" t="s">
+        <v>59</v>
+      </c>
+      <c r="I5" s="155">
+        <v>3906</v>
+      </c>
+      <c r="J5" s="156">
+        <v>44706</v>
+      </c>
+      <c r="K5" s="155">
+        <v>3906</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="89">
         <v>44692</v>
       </c>
-      <c r="C6" s="147">
+      <c r="C6" s="146">
         <v>44693</v>
       </c>
       <c r="D6" s="20">
@@ -4092,12 +4340,27 @@
         <f>E5+D6</f>
         <v>207018</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G6" s="153" t="s">
+        <v>60</v>
+      </c>
+      <c r="H6" s="154" t="s">
+        <v>61</v>
+      </c>
+      <c r="I6" s="155">
+        <v>33820.800000000003</v>
+      </c>
+      <c r="J6" s="156">
+        <v>44706</v>
+      </c>
+      <c r="K6" s="155">
+        <v>33820.800000000003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="89">
         <v>44693</v>
       </c>
-      <c r="C7" s="147">
+      <c r="C7" s="146">
         <v>44697</v>
       </c>
       <c r="D7" s="20">
@@ -4107,12 +4370,27 @@
         <f t="shared" ref="E7:E18" si="0">E6+D7</f>
         <v>247093</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G7" s="153" t="s">
+        <v>62</v>
+      </c>
+      <c r="H7" s="154" t="s">
+        <v>63</v>
+      </c>
+      <c r="I7" s="155">
+        <v>36277.25</v>
+      </c>
+      <c r="J7" s="156">
+        <v>44706</v>
+      </c>
+      <c r="K7" s="155">
+        <v>36277.25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="89">
         <v>44694</v>
       </c>
-      <c r="C8" s="147">
+      <c r="C8" s="146">
         <v>44697</v>
       </c>
       <c r="D8" s="20">
@@ -4122,12 +4400,27 @@
         <f t="shared" si="0"/>
         <v>303144</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G8" s="153" t="s">
+        <v>64</v>
+      </c>
+      <c r="H8" s="154" t="s">
+        <v>65</v>
+      </c>
+      <c r="I8" s="155">
+        <v>61531.34</v>
+      </c>
+      <c r="J8" s="156">
+        <v>44706</v>
+      </c>
+      <c r="K8" s="155">
+        <v>61531.34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="89">
         <v>44695</v>
       </c>
-      <c r="C9" s="147">
+      <c r="C9" s="146">
         <v>44697</v>
       </c>
       <c r="D9" s="20">
@@ -4137,15 +4430,27 @@
         <f t="shared" si="0"/>
         <v>346594</v>
       </c>
-      <c r="H9" s="123">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G9" s="153" t="s">
+        <v>64</v>
+      </c>
+      <c r="H9" s="154" t="s">
+        <v>66</v>
+      </c>
+      <c r="I9" s="155">
+        <v>12189.9</v>
+      </c>
+      <c r="J9" s="156">
+        <v>44706</v>
+      </c>
+      <c r="K9" s="155">
+        <v>12189.9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="89">
         <v>44696</v>
       </c>
-      <c r="C10" s="147">
+      <c r="C10" s="146">
         <v>44697</v>
       </c>
       <c r="D10" s="20">
@@ -4155,12 +4460,27 @@
         <f t="shared" si="0"/>
         <v>398929</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G10" s="153" t="s">
+        <v>67</v>
+      </c>
+      <c r="H10" s="154" t="s">
+        <v>68</v>
+      </c>
+      <c r="I10" s="155">
+        <v>64256.75</v>
+      </c>
+      <c r="J10" s="156">
+        <v>44706</v>
+      </c>
+      <c r="K10" s="155">
+        <v>64256.75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="89">
         <v>44697</v>
       </c>
-      <c r="C11" s="147">
+      <c r="C11" s="146">
         <v>44701</v>
       </c>
       <c r="D11" s="20">
@@ -4170,12 +4490,27 @@
         <f t="shared" si="0"/>
         <v>468120</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G11" s="153" t="s">
+        <v>69</v>
+      </c>
+      <c r="H11" s="154" t="s">
+        <v>70</v>
+      </c>
+      <c r="I11" s="155">
+        <v>53375.8</v>
+      </c>
+      <c r="J11" s="156">
+        <v>44706</v>
+      </c>
+      <c r="K11" s="155">
+        <v>53375.8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="89">
         <v>44698</v>
       </c>
-      <c r="C12" s="147">
+      <c r="C12" s="146">
         <v>44701</v>
       </c>
       <c r="D12" s="20">
@@ -4185,12 +4520,27 @@
         <f t="shared" si="0"/>
         <v>518275</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G12" s="153" t="s">
+        <v>71</v>
+      </c>
+      <c r="H12" s="154" t="s">
+        <v>72</v>
+      </c>
+      <c r="I12" s="155">
+        <v>126366.49</v>
+      </c>
+      <c r="J12" s="156">
+        <v>44706</v>
+      </c>
+      <c r="K12" s="155">
+        <v>126366.49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="89">
         <v>44699</v>
       </c>
-      <c r="C13" s="147">
+      <c r="C13" s="146">
         <v>44701</v>
       </c>
       <c r="D13" s="22">
@@ -4200,12 +4550,27 @@
         <f t="shared" si="0"/>
         <v>573502</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G13" s="153" t="s">
+        <v>71</v>
+      </c>
+      <c r="H13" s="154" t="s">
+        <v>73</v>
+      </c>
+      <c r="I13" s="155">
+        <v>6102</v>
+      </c>
+      <c r="J13" s="156">
+        <v>44706</v>
+      </c>
+      <c r="K13" s="155">
+        <v>6102</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="89">
         <v>44700</v>
       </c>
-      <c r="C14" s="147">
+      <c r="C14" s="146">
         <v>44701</v>
       </c>
       <c r="D14" s="20">
@@ -4215,12 +4580,27 @@
         <f t="shared" si="0"/>
         <v>620604</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G14" s="153" t="s">
+        <v>71</v>
+      </c>
+      <c r="H14" s="154" t="s">
+        <v>74</v>
+      </c>
+      <c r="I14" s="155">
+        <v>4812</v>
+      </c>
+      <c r="J14" s="156">
+        <v>44706</v>
+      </c>
+      <c r="K14" s="155">
+        <v>4812</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="89">
         <v>44701</v>
       </c>
-      <c r="C15" s="147">
+      <c r="C15" s="146">
         <v>44704</v>
       </c>
       <c r="D15" s="20">
@@ -4230,12 +4610,27 @@
         <f t="shared" si="0"/>
         <v>713738</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G15" s="153" t="s">
+        <v>75</v>
+      </c>
+      <c r="H15" s="154" t="s">
+        <v>76</v>
+      </c>
+      <c r="I15" s="155">
+        <v>10160.6</v>
+      </c>
+      <c r="J15" s="156">
+        <v>44706</v>
+      </c>
+      <c r="K15" s="155">
+        <v>10160.6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="89">
         <v>44702</v>
       </c>
-      <c r="C16" s="147">
+      <c r="C16" s="146">
         <v>44704</v>
       </c>
       <c r="D16" s="20">
@@ -4245,12 +4640,27 @@
         <f t="shared" si="0"/>
         <v>736046</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G16" s="153" t="s">
+        <v>75</v>
+      </c>
+      <c r="H16" s="154" t="s">
+        <v>77</v>
+      </c>
+      <c r="I16" s="155">
+        <v>75337.5</v>
+      </c>
+      <c r="J16" s="156">
+        <v>44706</v>
+      </c>
+      <c r="K16" s="155">
+        <v>75337.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="89">
         <v>44703</v>
       </c>
-      <c r="C17" s="147">
+      <c r="C17" s="146">
         <v>44704</v>
       </c>
       <c r="D17" s="20">
@@ -4260,299 +4670,464 @@
         <f t="shared" si="0"/>
         <v>759582</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G17" s="153" t="s">
+        <v>78</v>
+      </c>
+      <c r="H17" s="154" t="s">
+        <v>79</v>
+      </c>
+      <c r="I17" s="155">
+        <v>29920.44</v>
+      </c>
+      <c r="J17" s="156">
+        <v>44706</v>
+      </c>
+      <c r="K17" s="155">
+        <v>29920.44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="89"/>
-      <c r="C18" s="147"/>
+      <c r="C18" s="146"/>
       <c r="D18" s="20"/>
-      <c r="E18" s="20">
+      <c r="E18" s="165">
         <f t="shared" si="0"/>
         <v>759582</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="30"/>
-      <c r="C19" s="147"/>
-      <c r="D19" s="138"/>
-      <c r="E19" s="138"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G18" s="153" t="s">
+        <v>80</v>
+      </c>
+      <c r="H18" s="154" t="s">
+        <v>81</v>
+      </c>
+      <c r="I18" s="155">
+        <v>72246.7</v>
+      </c>
+      <c r="J18" s="156">
+        <v>44706</v>
+      </c>
+      <c r="K18" s="155">
+        <v>72246.7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="159"/>
+      <c r="C19" s="160"/>
+      <c r="D19" s="161"/>
+      <c r="E19" s="161"/>
+      <c r="G19" s="153" t="s">
+        <v>80</v>
+      </c>
+      <c r="H19" s="154" t="s">
+        <v>82</v>
+      </c>
+      <c r="I19" s="155">
+        <v>3036</v>
+      </c>
+      <c r="J19" s="156">
+        <v>44706</v>
+      </c>
+      <c r="K19" s="155">
+        <v>3036</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="21" x14ac:dyDescent="0.35">
       <c r="A20" s="130"/>
-      <c r="B20" s="110"/>
-      <c r="C20" s="148"/>
-      <c r="D20" s="60"/>
-      <c r="E20" s="60"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B20" s="162" t="s">
+        <v>87</v>
+      </c>
+      <c r="C20" s="163"/>
+      <c r="D20" s="164"/>
+      <c r="E20" s="164"/>
+      <c r="G20" s="153" t="s">
+        <v>83</v>
+      </c>
+      <c r="H20" s="154" t="s">
+        <v>84</v>
+      </c>
+      <c r="I20" s="155">
+        <v>1627.2</v>
+      </c>
+      <c r="J20" s="156">
+        <v>44706</v>
+      </c>
+      <c r="K20" s="155">
+        <v>1627.2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="130"/>
       <c r="B21" s="110"/>
-      <c r="C21" s="148"/>
+      <c r="C21" s="147"/>
       <c r="D21" s="60"/>
       <c r="E21" s="60"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G21" s="153" t="s">
+        <v>83</v>
+      </c>
+      <c r="H21" s="154" t="s">
+        <v>85</v>
+      </c>
+      <c r="I21" s="155">
+        <v>1238.8</v>
+      </c>
+      <c r="J21" s="156">
+        <v>44706</v>
+      </c>
+      <c r="K21" s="155">
+        <v>1238.8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="130"/>
       <c r="B22" s="110"/>
-      <c r="C22" s="148"/>
+      <c r="C22" s="147"/>
       <c r="D22" s="60"/>
       <c r="E22" s="60"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="G22" s="153" t="s">
+        <v>83</v>
+      </c>
+      <c r="H22" s="154" t="s">
+        <v>86</v>
+      </c>
+      <c r="I22" s="155">
+        <v>62762.55</v>
+      </c>
+      <c r="J22" s="156">
+        <v>44706</v>
+      </c>
+      <c r="K22" s="157">
+        <v>50646.16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="130"/>
       <c r="B23" s="110"/>
-      <c r="C23" s="148"/>
+      <c r="C23" s="147"/>
       <c r="D23" s="60"/>
       <c r="E23" s="60"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="K23" s="158">
+        <f>SUM(K2:K22)</f>
+        <v>759581.99999999988</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="130"/>
       <c r="B24" s="110"/>
-      <c r="C24" s="148"/>
+      <c r="C24" s="147"/>
       <c r="D24" s="60"/>
       <c r="E24" s="60"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="130"/>
       <c r="B25" s="110"/>
-      <c r="C25" s="148"/>
+      <c r="C25" s="147"/>
       <c r="D25" s="60"/>
       <c r="E25" s="60"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="130"/>
-      <c r="B26" s="110"/>
-      <c r="C26" s="148"/>
-      <c r="D26" s="60"/>
-      <c r="E26" s="60"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="130"/>
-      <c r="B27" s="110"/>
-      <c r="C27" s="148"/>
-      <c r="D27" s="60"/>
-      <c r="E27" s="60"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="130"/>
-      <c r="B28" s="110"/>
-      <c r="C28" s="148"/>
-      <c r="D28" s="60"/>
-      <c r="E28" s="60"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" s="130"/>
-      <c r="B29" s="110"/>
-      <c r="C29" s="148"/>
-      <c r="D29" s="60"/>
-      <c r="E29" s="60"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" s="130"/>
-      <c r="B30" s="110"/>
-      <c r="C30" s="148"/>
-      <c r="D30" s="60"/>
-      <c r="E30" s="60"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" s="130"/>
-      <c r="B31" s="110"/>
-      <c r="C31" s="148"/>
-      <c r="D31" s="60"/>
-      <c r="E31" s="60"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" s="130"/>
-      <c r="B32" s="110"/>
-      <c r="C32" s="148"/>
-      <c r="D32" s="60"/>
-      <c r="E32" s="60"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" s="130"/>
-      <c r="B33" s="110"/>
-      <c r="C33" s="148"/>
-      <c r="D33" s="60"/>
-      <c r="E33" s="60"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" s="130"/>
-      <c r="B34" s="110"/>
-      <c r="C34" s="148"/>
-      <c r="D34" s="60"/>
-      <c r="E34" s="60"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" s="130"/>
-      <c r="B35" s="110"/>
-      <c r="C35" s="148"/>
-      <c r="D35" s="60"/>
-      <c r="E35" s="60"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A36" s="130"/>
-      <c r="B36" s="110"/>
-      <c r="C36" s="148"/>
-      <c r="D36" s="60"/>
-      <c r="E36" s="60"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37" s="130"/>
-      <c r="B37" s="110"/>
-      <c r="C37" s="148"/>
-      <c r="D37" s="60"/>
-      <c r="E37" s="60"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A38" s="130"/>
-      <c r="B38" s="110"/>
-      <c r="C38" s="148"/>
-      <c r="D38" s="60"/>
-      <c r="E38" s="60"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A39" s="130"/>
-      <c r="B39" s="110"/>
-      <c r="C39" s="148"/>
-      <c r="D39" s="60"/>
-      <c r="E39" s="60"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A40" s="130"/>
-      <c r="B40" s="110"/>
-      <c r="C40" s="148"/>
-      <c r="D40" s="60"/>
-      <c r="E40" s="60"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41" s="130"/>
-      <c r="B41" s="110"/>
-      <c r="C41" s="148"/>
-      <c r="D41" s="60"/>
-      <c r="E41" s="60"/>
+    <row r="26" spans="1:11" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="179" t="s">
+        <v>43</v>
+      </c>
+      <c r="B26" s="180"/>
+      <c r="C26" s="180"/>
+      <c r="D26" s="180"/>
+      <c r="E26" s="180"/>
+    </row>
+    <row r="27" spans="1:11" ht="33.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B27" s="141" t="s">
+        <v>44</v>
+      </c>
+      <c r="C27" s="144" t="s">
+        <v>45</v>
+      </c>
+      <c r="D27" s="149" t="s">
+        <v>2</v>
+      </c>
+      <c r="E27" s="143" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="139">
+        <v>44704</v>
+      </c>
+      <c r="C28" s="145"/>
+      <c r="D28" s="140"/>
+      <c r="E28" s="140">
+        <f>D28</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="139">
+        <v>44705</v>
+      </c>
+      <c r="C29" s="146"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="20">
+        <f>E28+D29</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="139">
+        <v>44706</v>
+      </c>
+      <c r="C30" s="146"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20">
+        <f>E29+D30</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="139">
+        <v>44707</v>
+      </c>
+      <c r="C31" s="146"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="20">
+        <f t="shared" ref="E31:E42" si="1">E30+D31</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="139">
+        <v>44708</v>
+      </c>
+      <c r="C32" s="146"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="139">
+        <v>44709</v>
+      </c>
+      <c r="C33" s="146"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="139">
+        <v>44710</v>
+      </c>
+      <c r="C34" s="146"/>
+      <c r="D34" s="20"/>
+      <c r="E34" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="139">
+        <v>44711</v>
+      </c>
+      <c r="C35" s="146"/>
+      <c r="D35" s="20"/>
+      <c r="E35" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="139">
+        <v>44712</v>
+      </c>
+      <c r="C36" s="146"/>
+      <c r="D36" s="20"/>
+      <c r="E36" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="139">
+        <v>44713</v>
+      </c>
+      <c r="C37" s="146"/>
+      <c r="D37" s="22"/>
+      <c r="E37" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="139">
+        <v>44714</v>
+      </c>
+      <c r="C38" s="146"/>
+      <c r="D38" s="20"/>
+      <c r="E38" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="139">
+        <v>44715</v>
+      </c>
+      <c r="C39" s="146"/>
+      <c r="D39" s="20"/>
+      <c r="E39" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="139">
+        <v>44716</v>
+      </c>
+      <c r="C40" s="146"/>
+      <c r="D40" s="20"/>
+      <c r="E40" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="139">
+        <v>44717</v>
+      </c>
+      <c r="C41" s="146"/>
+      <c r="D41" s="20"/>
+      <c r="E41" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A42" s="130"/>
-      <c r="B42" s="110"/>
-      <c r="C42" s="148"/>
-      <c r="D42" s="60"/>
-      <c r="E42" s="60"/>
+      <c r="B42" s="139">
+        <v>44718</v>
+      </c>
+      <c r="C42" s="146"/>
+      <c r="D42" s="20"/>
+      <c r="E42" s="165">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="130"/>
       <c r="B43" s="110"/>
-      <c r="C43" s="148"/>
+      <c r="C43" s="147"/>
       <c r="D43" s="60"/>
       <c r="E43" s="60"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="130"/>
       <c r="B44" s="110"/>
-      <c r="C44" s="148"/>
+      <c r="C44" s="147"/>
       <c r="D44" s="60"/>
       <c r="E44" s="60"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="130"/>
       <c r="B45" s="110"/>
-      <c r="C45" s="148"/>
-      <c r="D45" s="143"/>
+      <c r="C45" s="147"/>
+      <c r="D45" s="142"/>
       <c r="E45" s="60"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="130"/>
       <c r="B46" s="110"/>
-      <c r="C46" s="148"/>
+      <c r="C46" s="147"/>
       <c r="D46" s="60"/>
       <c r="E46" s="60"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="130"/>
       <c r="B47" s="110"/>
-      <c r="C47" s="148"/>
+      <c r="C47" s="147"/>
       <c r="D47" s="60"/>
       <c r="E47" s="60"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="130"/>
       <c r="B48" s="110"/>
-      <c r="C48" s="148"/>
+      <c r="C48" s="147"/>
       <c r="D48" s="60"/>
       <c r="E48" s="60"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="130"/>
       <c r="B49" s="110"/>
-      <c r="C49" s="148"/>
+      <c r="C49" s="147"/>
       <c r="D49" s="60"/>
       <c r="E49" s="60"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="130"/>
       <c r="B50" s="110"/>
-      <c r="C50" s="148"/>
+      <c r="C50" s="147"/>
       <c r="D50" s="60"/>
       <c r="E50" s="60"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="130"/>
       <c r="B51" s="110"/>
-      <c r="C51" s="148"/>
+      <c r="C51" s="147"/>
       <c r="D51" s="60"/>
       <c r="E51" s="60"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="130"/>
       <c r="B52" s="110"/>
-      <c r="C52" s="148"/>
+      <c r="C52" s="147"/>
       <c r="D52" s="60"/>
       <c r="E52" s="60"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="130"/>
       <c r="B53" s="110"/>
-      <c r="C53" s="148"/>
+      <c r="C53" s="147"/>
       <c r="D53" s="62"/>
       <c r="E53" s="60"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="130"/>
       <c r="B54" s="110"/>
-      <c r="C54" s="148"/>
+      <c r="C54" s="147"/>
       <c r="D54" s="60"/>
       <c r="E54" s="60"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="130"/>
       <c r="B55" s="110"/>
-      <c r="C55" s="148"/>
+      <c r="C55" s="147"/>
       <c r="D55" s="60"/>
       <c r="E55" s="60"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" s="130"/>
       <c r="B56" s="110"/>
-      <c r="C56" s="148"/>
+      <c r="C56" s="147"/>
       <c r="D56" s="60"/>
       <c r="E56" s="60"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="130"/>
       <c r="B57" s="110"/>
-      <c r="C57" s="148"/>
+      <c r="C57" s="147"/>
       <c r="D57" s="60"/>
       <c r="E57" s="60"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" s="130"/>
       <c r="B58" s="110"/>
-      <c r="C58" s="148"/>
+      <c r="C58" s="147"/>
       <c r="D58" s="60"/>
       <c r="E58" s="60"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="130"/>
       <c r="B59" s="110"/>
-      <c r="C59" s="148"/>
+      <c r="C59" s="147"/>
       <c r="D59" s="60"/>
       <c r="E59" s="60"/>
     </row>
@@ -4562,7 +5137,7 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D61" s="131"/>
-      <c r="E61" s="139"/>
+      <c r="E61" s="138"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D62" s="131"/>
@@ -4572,11 +5147,14 @@
   <sortState ref="B3:G63">
     <sortCondition ref="D3:D63"/>
   </sortState>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A26:E26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -4604,27 +5182,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="169" t="s">
+      <c r="A1" s="181" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="170"/>
-      <c r="C1" s="170"/>
-      <c r="D1" s="170"/>
-      <c r="E1" s="170"/>
-      <c r="F1" s="170"/>
-      <c r="G1" s="170"/>
+      <c r="B1" s="182"/>
+      <c r="C1" s="182"/>
+      <c r="D1" s="182"/>
+      <c r="E1" s="182"/>
+      <c r="F1" s="182"/>
+      <c r="G1" s="182"/>
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="171" t="s">
+      <c r="A2" s="183" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="171"/>
-      <c r="C2" s="171"/>
-      <c r="D2" s="171"/>
-      <c r="E2" s="171"/>
-      <c r="F2" s="171"/>
-      <c r="G2" s="171"/>
+      <c r="B2" s="183"/>
+      <c r="C2" s="183"/>
+      <c r="D2" s="183"/>
+      <c r="E2" s="183"/>
+      <c r="F2" s="183"/>
+      <c r="G2" s="183"/>
       <c r="H2" s="5"/>
       <c r="I2" s="2"/>
     </row>
@@ -4819,11 +5397,11 @@
         <v>161427</v>
       </c>
       <c r="F11" s="21"/>
-      <c r="G11" s="172">
+      <c r="G11" s="184">
         <f>SUM(H4:H10)</f>
         <v>48874</v>
       </c>
-      <c r="H11" s="173"/>
+      <c r="H11" s="185"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="12"/>
@@ -6198,11 +6776,11 @@
         <v>76469.81</v>
       </c>
       <c r="F81" s="61"/>
-      <c r="G81" s="174">
+      <c r="G81" s="186">
         <f>SUM(H67:H80)</f>
         <v>76469.81</v>
       </c>
-      <c r="H81" s="175"/>
+      <c r="H81" s="187"/>
     </row>
     <row r="82" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="23"/>
@@ -6290,12 +6868,12 @@
       <c r="B88" s="37"/>
       <c r="C88" s="38"/>
       <c r="D88" s="2"/>
-      <c r="E88" s="155">
+      <c r="E88" s="167">
         <f>E84-G84</f>
         <v>1332859.9100000001</v>
       </c>
-      <c r="F88" s="156"/>
-      <c r="G88" s="157"/>
+      <c r="F88" s="168"/>
+      <c r="G88" s="169"/>
       <c r="H88" s="44"/>
       <c r="I88" s="2"/>
     </row>
@@ -6312,11 +6890,11 @@
       <c r="B90" s="37"/>
       <c r="C90" s="38"/>
       <c r="D90" s="2"/>
-      <c r="E90" s="158" t="s">
+      <c r="E90" s="170" t="s">
         <v>8</v>
       </c>
-      <c r="F90" s="158"/>
-      <c r="G90" s="158"/>
+      <c r="F90" s="170"/>
+      <c r="G90" s="170"/>
       <c r="I90" s="2"/>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
@@ -6461,25 +7039,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="159" t="s">
+      <c r="B1" s="171" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="160"/>
-      <c r="D1" s="160"/>
-      <c r="E1" s="160"/>
-      <c r="F1" s="160"/>
-      <c r="G1" s="161"/>
+      <c r="C1" s="172"/>
+      <c r="D1" s="172"/>
+      <c r="E1" s="172"/>
+      <c r="F1" s="172"/>
+      <c r="G1" s="173"/>
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
-      <c r="B2" s="154" t="s">
+      <c r="B2" s="166" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="154"/>
-      <c r="D2" s="154"/>
-      <c r="E2" s="154"/>
-      <c r="F2" s="154"/>
+      <c r="C2" s="166"/>
+      <c r="D2" s="166"/>
+      <c r="E2" s="166"/>
+      <c r="F2" s="166"/>
       <c r="G2" s="4"/>
       <c r="H2" s="5"/>
       <c r="I2" s="2"/>
@@ -7371,12 +7949,12 @@
       <c r="B52" s="37"/>
       <c r="C52" s="38"/>
       <c r="D52" s="2"/>
-      <c r="E52" s="155">
+      <c r="E52" s="167">
         <f>E48-G48</f>
         <v>734621</v>
       </c>
-      <c r="F52" s="156"/>
-      <c r="G52" s="157"/>
+      <c r="F52" s="168"/>
+      <c r="G52" s="169"/>
       <c r="I52" s="2"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
@@ -7392,11 +7970,11 @@
       <c r="B54" s="37"/>
       <c r="C54" s="38"/>
       <c r="D54" s="2"/>
-      <c r="E54" s="158" t="s">
+      <c r="E54" s="170" t="s">
         <v>8</v>
       </c>
-      <c r="F54" s="158"/>
-      <c r="G54" s="158"/>
+      <c r="F54" s="170"/>
+      <c r="G54" s="170"/>
       <c r="I54" s="2"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
@@ -7552,25 +8130,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="159" t="s">
+      <c r="B1" s="171" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="160"/>
-      <c r="D1" s="160"/>
-      <c r="E1" s="160"/>
-      <c r="F1" s="160"/>
-      <c r="G1" s="161"/>
+      <c r="C1" s="172"/>
+      <c r="D1" s="172"/>
+      <c r="E1" s="172"/>
+      <c r="F1" s="172"/>
+      <c r="G1" s="173"/>
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
-      <c r="B2" s="154" t="s">
+      <c r="B2" s="166" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="154"/>
-      <c r="D2" s="154"/>
-      <c r="E2" s="154"/>
-      <c r="F2" s="154"/>
+      <c r="C2" s="166"/>
+      <c r="D2" s="166"/>
+      <c r="E2" s="166"/>
+      <c r="F2" s="166"/>
       <c r="G2" s="4"/>
       <c r="H2" s="5"/>
       <c r="I2" s="2"/>
@@ -9300,12 +9878,12 @@
       <c r="B76" s="37"/>
       <c r="C76" s="38"/>
       <c r="D76" s="2"/>
-      <c r="E76" s="155">
+      <c r="E76" s="167">
         <f>E72-G72</f>
         <v>0</v>
       </c>
-      <c r="F76" s="156"/>
-      <c r="G76" s="157"/>
+      <c r="F76" s="168"/>
+      <c r="G76" s="169"/>
       <c r="I76" s="2"/>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
@@ -9321,11 +9899,11 @@
       <c r="B78" s="37"/>
       <c r="C78" s="38"/>
       <c r="D78" s="2"/>
-      <c r="E78" s="158" t="s">
+      <c r="E78" s="170" t="s">
         <v>8</v>
       </c>
-      <c r="F78" s="158"/>
-      <c r="G78" s="158"/>
+      <c r="F78" s="170"/>
+      <c r="G78" s="170"/>
       <c r="I78" s="2"/>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
@@ -9466,25 +10044,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="159" t="s">
+      <c r="B1" s="171" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="160"/>
-      <c r="D1" s="160"/>
-      <c r="E1" s="160"/>
-      <c r="F1" s="160"/>
-      <c r="G1" s="161"/>
+      <c r="C1" s="172"/>
+      <c r="D1" s="172"/>
+      <c r="E1" s="172"/>
+      <c r="F1" s="172"/>
+      <c r="G1" s="173"/>
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
-      <c r="B2" s="154" t="s">
+      <c r="B2" s="166" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="154"/>
-      <c r="D2" s="154"/>
-      <c r="E2" s="154"/>
-      <c r="F2" s="154"/>
+      <c r="C2" s="166"/>
+      <c r="D2" s="166"/>
+      <c r="E2" s="166"/>
+      <c r="F2" s="166"/>
       <c r="G2" s="4"/>
       <c r="H2" s="5"/>
       <c r="I2" s="2"/>
@@ -10333,12 +10911,12 @@
       <c r="B41" s="37"/>
       <c r="C41" s="38"/>
       <c r="D41" s="2"/>
-      <c r="E41" s="155">
+      <c r="E41" s="167">
         <f>E37-G37</f>
         <v>0</v>
       </c>
-      <c r="F41" s="156"/>
-      <c r="G41" s="157"/>
+      <c r="F41" s="168"/>
+      <c r="G41" s="169"/>
       <c r="I41" s="2"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -10354,11 +10932,11 @@
       <c r="B43" s="37"/>
       <c r="C43" s="38"/>
       <c r="D43" s="2"/>
-      <c r="E43" s="158" t="s">
+      <c r="E43" s="170" t="s">
         <v>8</v>
       </c>
-      <c r="F43" s="158"/>
-      <c r="G43" s="158"/>
+      <c r="F43" s="170"/>
+      <c r="G43" s="170"/>
       <c r="I43" s="2"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
@@ -10502,25 +11080,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="162" t="s">
+      <c r="B1" s="174" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="163"/>
-      <c r="D1" s="163"/>
-      <c r="E1" s="163"/>
-      <c r="F1" s="163"/>
-      <c r="G1" s="164"/>
+      <c r="C1" s="175"/>
+      <c r="D1" s="175"/>
+      <c r="E1" s="175"/>
+      <c r="F1" s="175"/>
+      <c r="G1" s="176"/>
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
-      <c r="B2" s="154" t="s">
+      <c r="B2" s="166" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="154"/>
-      <c r="D2" s="154"/>
-      <c r="E2" s="154"/>
-      <c r="F2" s="154"/>
+      <c r="C2" s="166"/>
+      <c r="D2" s="166"/>
+      <c r="E2" s="166"/>
+      <c r="F2" s="166"/>
       <c r="G2" s="4"/>
       <c r="H2" s="5"/>
       <c r="I2" s="2"/>
@@ -11860,12 +12438,12 @@
       <c r="B60" s="37"/>
       <c r="C60" s="38"/>
       <c r="D60" s="2"/>
-      <c r="E60" s="155">
+      <c r="E60" s="167">
         <f>E56-G56</f>
         <v>0</v>
       </c>
-      <c r="F60" s="156"/>
-      <c r="G60" s="157"/>
+      <c r="F60" s="168"/>
+      <c r="G60" s="169"/>
       <c r="I60" s="2"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
@@ -11881,11 +12459,11 @@
       <c r="B62" s="37"/>
       <c r="C62" s="38"/>
       <c r="D62" s="2"/>
-      <c r="E62" s="158" t="s">
+      <c r="E62" s="170" t="s">
         <v>8</v>
       </c>
-      <c r="F62" s="158"/>
-      <c r="G62" s="158"/>
+      <c r="F62" s="170"/>
+      <c r="G62" s="170"/>
       <c r="I62" s="2"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
@@ -12026,25 +12604,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="162" t="s">
+      <c r="B1" s="174" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="163"/>
-      <c r="D1" s="163"/>
-      <c r="E1" s="163"/>
-      <c r="F1" s="163"/>
-      <c r="G1" s="164"/>
+      <c r="C1" s="175"/>
+      <c r="D1" s="175"/>
+      <c r="E1" s="175"/>
+      <c r="F1" s="175"/>
+      <c r="G1" s="176"/>
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
-      <c r="B2" s="154" t="s">
+      <c r="B2" s="166" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="154"/>
-      <c r="D2" s="154"/>
-      <c r="E2" s="154"/>
-      <c r="F2" s="154"/>
+      <c r="C2" s="166"/>
+      <c r="D2" s="166"/>
+      <c r="E2" s="166"/>
+      <c r="F2" s="166"/>
       <c r="G2" s="4"/>
       <c r="H2" s="5"/>
       <c r="I2" s="2"/>
@@ -13445,12 +14023,12 @@
       <c r="B61" s="37"/>
       <c r="C61" s="38"/>
       <c r="D61" s="2"/>
-      <c r="E61" s="155">
+      <c r="E61" s="167">
         <f>E57-G57</f>
         <v>0</v>
       </c>
-      <c r="F61" s="156"/>
-      <c r="G61" s="157"/>
+      <c r="F61" s="168"/>
+      <c r="G61" s="169"/>
       <c r="I61" s="2"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
@@ -13466,11 +14044,11 @@
       <c r="B63" s="37"/>
       <c r="C63" s="38"/>
       <c r="D63" s="2"/>
-      <c r="E63" s="158" t="s">
+      <c r="E63" s="170" t="s">
         <v>8</v>
       </c>
-      <c r="F63" s="158"/>
-      <c r="G63" s="158"/>
+      <c r="F63" s="170"/>
+      <c r="G63" s="170"/>
       <c r="I63" s="2"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
@@ -13611,25 +14189,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="162" t="s">
+      <c r="B1" s="174" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="163"/>
-      <c r="D1" s="163"/>
-      <c r="E1" s="163"/>
-      <c r="F1" s="163"/>
-      <c r="G1" s="164"/>
+      <c r="C1" s="175"/>
+      <c r="D1" s="175"/>
+      <c r="E1" s="175"/>
+      <c r="F1" s="175"/>
+      <c r="G1" s="176"/>
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
-      <c r="B2" s="154" t="s">
+      <c r="B2" s="166" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="154"/>
-      <c r="D2" s="154"/>
-      <c r="E2" s="154"/>
-      <c r="F2" s="154"/>
+      <c r="C2" s="166"/>
+      <c r="D2" s="166"/>
+      <c r="E2" s="166"/>
+      <c r="F2" s="166"/>
       <c r="G2" s="4"/>
       <c r="H2" s="5"/>
       <c r="I2" s="2"/>
@@ -15079,12 +15657,12 @@
       <c r="B64" s="37"/>
       <c r="C64" s="38"/>
       <c r="D64" s="2"/>
-      <c r="E64" s="155">
+      <c r="E64" s="167">
         <f>E60-G60</f>
         <v>0</v>
       </c>
-      <c r="F64" s="156"/>
-      <c r="G64" s="157"/>
+      <c r="F64" s="168"/>
+      <c r="G64" s="169"/>
       <c r="I64" s="2"/>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
@@ -15100,11 +15678,11 @@
       <c r="B66" s="37"/>
       <c r="C66" s="38"/>
       <c r="D66" s="2"/>
-      <c r="E66" s="158" t="s">
+      <c r="E66" s="170" t="s">
         <v>8</v>
       </c>
-      <c r="F66" s="158"/>
-      <c r="G66" s="158"/>
+      <c r="F66" s="170"/>
+      <c r="G66" s="170"/>
       <c r="I66" s="2"/>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
@@ -15245,25 +15823,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="162" t="s">
+      <c r="B1" s="174" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="163"/>
-      <c r="D1" s="163"/>
-      <c r="E1" s="163"/>
-      <c r="F1" s="163"/>
-      <c r="G1" s="164"/>
+      <c r="C1" s="175"/>
+      <c r="D1" s="175"/>
+      <c r="E1" s="175"/>
+      <c r="F1" s="175"/>
+      <c r="G1" s="176"/>
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
-      <c r="B2" s="154" t="s">
+      <c r="B2" s="166" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="154"/>
-      <c r="D2" s="154"/>
-      <c r="E2" s="154"/>
-      <c r="F2" s="154"/>
+      <c r="C2" s="166"/>
+      <c r="D2" s="166"/>
+      <c r="E2" s="166"/>
+      <c r="F2" s="166"/>
       <c r="G2" s="4"/>
       <c r="H2" s="5"/>
       <c r="I2" s="2"/>
@@ -16664,12 +17242,12 @@
       <c r="B65" s="37"/>
       <c r="C65" s="38"/>
       <c r="D65" s="2"/>
-      <c r="E65" s="155">
+      <c r="E65" s="167">
         <f>E61-G61</f>
         <v>210191</v>
       </c>
-      <c r="F65" s="156"/>
-      <c r="G65" s="157"/>
+      <c r="F65" s="168"/>
+      <c r="G65" s="169"/>
       <c r="I65" s="2"/>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
@@ -16685,11 +17263,11 @@
       <c r="B67" s="37"/>
       <c r="C67" s="38"/>
       <c r="D67" s="2"/>
-      <c r="E67" s="158" t="s">
+      <c r="E67" s="170" t="s">
         <v>8</v>
       </c>
-      <c r="F67" s="158"/>
-      <c r="G67" s="158"/>
+      <c r="F67" s="170"/>
+      <c r="G67" s="170"/>
       <c r="I67" s="2"/>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
@@ -16853,8 +17431,8 @@
   </sheetPr>
   <dimension ref="A1:I80"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -16871,25 +17449,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="162" t="s">
+      <c r="B1" s="174" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="163"/>
-      <c r="D1" s="163"/>
-      <c r="E1" s="163"/>
-      <c r="F1" s="163"/>
-      <c r="G1" s="164"/>
+      <c r="C1" s="175"/>
+      <c r="D1" s="175"/>
+      <c r="E1" s="175"/>
+      <c r="F1" s="175"/>
+      <c r="G1" s="176"/>
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
-      <c r="B2" s="154" t="s">
+      <c r="B2" s="166" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="154"/>
-      <c r="D2" s="154"/>
-      <c r="E2" s="154"/>
-      <c r="F2" s="154"/>
+      <c r="C2" s="166"/>
+      <c r="D2" s="166"/>
+      <c r="E2" s="166"/>
+      <c r="F2" s="166"/>
       <c r="G2" s="4"/>
       <c r="H2" s="5"/>
       <c r="I2" s="2"/>
@@ -17016,7 +17594,7 @@
         <v>344</v>
       </c>
       <c r="C8" s="90"/>
-      <c r="D8" s="151" t="s">
+      <c r="D8" s="150" t="s">
         <v>41</v>
       </c>
       <c r="E8" s="20">
@@ -17209,7 +17787,7 @@
         <v>353</v>
       </c>
       <c r="C17" s="25"/>
-      <c r="D17" s="151" t="s">
+      <c r="D17" s="150" t="s">
         <v>52</v>
       </c>
       <c r="E17" s="20">
@@ -17335,7 +17913,7 @@
         <v>359</v>
       </c>
       <c r="C23" s="24"/>
-      <c r="D23" s="152" t="s">
+      <c r="D23" s="151" t="s">
         <v>41</v>
       </c>
       <c r="E23" s="20">
@@ -17356,7 +17934,7 @@
         <v>360</v>
       </c>
       <c r="C24" s="24"/>
-      <c r="D24" s="152" t="s">
+      <c r="D24" s="151" t="s">
         <v>53</v>
       </c>
       <c r="E24" s="20">
@@ -17374,33 +17952,49 @@
       </c>
     </row>
     <row r="25" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="12"/>
+      <c r="A25" s="12">
+        <v>44700</v>
+      </c>
       <c r="B25" s="13">
         <v>361</v>
       </c>
       <c r="C25" s="24"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="20"/>
-      <c r="F25" s="21"/>
-      <c r="G25" s="22"/>
+      <c r="D25" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="E25" s="20">
+        <v>8257</v>
+      </c>
+      <c r="F25" s="21">
+        <v>44700</v>
+      </c>
+      <c r="G25" s="22">
+        <v>8257</v>
+      </c>
       <c r="H25" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="12"/>
+      <c r="A26" s="12">
+        <v>44700</v>
+      </c>
       <c r="B26" s="13">
         <v>362</v>
       </c>
       <c r="C26" s="24"/>
-      <c r="D26" s="19"/>
-      <c r="E26" s="20"/>
+      <c r="D26" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="E26" s="20">
+        <v>27353</v>
+      </c>
       <c r="F26" s="21"/>
       <c r="G26" s="22"/>
       <c r="H26" s="18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>27353</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -17917,16 +18511,16 @@
       <c r="D61" s="2"/>
       <c r="E61" s="39">
         <f>SUM(E4:E60)</f>
-        <v>389692</v>
+        <v>425302</v>
       </c>
       <c r="F61" s="39"/>
       <c r="G61" s="39">
         <f>SUM(G4:G60)</f>
-        <v>11377</v>
+        <v>19634</v>
       </c>
       <c r="H61" s="40">
         <f>SUM(H4:H60)</f>
-        <v>378315</v>
+        <v>405668</v>
       </c>
       <c r="I61" s="2"/>
     </row>
@@ -17968,12 +18562,12 @@
       <c r="B65" s="37"/>
       <c r="C65" s="38"/>
       <c r="D65" s="2"/>
-      <c r="E65" s="155">
+      <c r="E65" s="167">
         <f>E61-G61</f>
-        <v>378315</v>
-      </c>
-      <c r="F65" s="156"/>
-      <c r="G65" s="157"/>
+        <v>405668</v>
+      </c>
+      <c r="F65" s="168"/>
+      <c r="G65" s="169"/>
       <c r="I65" s="2"/>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
@@ -17989,11 +18583,11 @@
       <c r="B67" s="37"/>
       <c r="C67" s="38"/>
       <c r="D67" s="2"/>
-      <c r="E67" s="158" t="s">
+      <c r="E67" s="170" t="s">
         <v>8</v>
       </c>
-      <c r="F67" s="158"/>
-      <c r="G67" s="158"/>
+      <c r="F67" s="170"/>
+      <c r="G67" s="170"/>
       <c r="I67" s="2"/>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>